<commit_message>
This is the sixth commit.
</commit_message>
<xml_diff>
--- a/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
+++ b/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -44,13 +44,85 @@
   </si>
   <si>
     <t>Prod123</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>mobilePhoneNumber</t>
+  </si>
+  <si>
+    <t>StudentOne</t>
+  </si>
+  <si>
+    <t>TeacherOne</t>
+  </si>
+  <si>
+    <t>Password1</t>
+  </si>
+  <si>
+    <t>Password2</t>
+  </si>
+  <si>
+    <t>Password3</t>
+  </si>
+  <si>
+    <t>Password4</t>
+  </si>
+  <si>
+    <t>Password5</t>
+  </si>
+  <si>
+    <t>Password6</t>
+  </si>
+  <si>
+    <t>Password7</t>
+  </si>
+  <si>
+    <t>Password8</t>
+  </si>
+  <si>
+    <t>Password9</t>
+  </si>
+  <si>
+    <t>Password10</t>
+  </si>
+  <si>
+    <t>FirstOne</t>
+  </si>
+  <si>
+    <t>LastOne</t>
+  </si>
+  <si>
+    <t>MiddleOne</t>
+  </si>
+  <si>
+    <t>ThreeTwoOne</t>
+  </si>
+  <si>
+    <t>TallestOne</t>
+  </si>
+  <si>
+    <t>ShortestOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,8 +130,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -72,8 +159,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -81,13 +186,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,13 +503,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="M6" sqref="M4:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.90625" customWidth="1"/>
-    <col min="2" max="2" width="44.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -419,17 +551,206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" style="2" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5">
+        <v>9876</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="5">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="5">
+        <v>9876543211</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
This is sixth commit.
</commit_message>
<xml_diff>
--- a/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
+++ b/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="SignUpTest" sheetId="2" r:id="rId2"/>
+    <sheet name="AddingItemToCart" sheetId="4" r:id="rId3"/>
+    <sheet name="NavigateCheckoutAndDummyPayment" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
   <si>
     <t>Username</t>
   </si>
@@ -116,13 +119,241 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>firstName2</t>
+  </si>
+  <si>
+    <t>lastName2</t>
+  </si>
+  <si>
+    <t>address2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>useremailaddress</t>
+  </si>
+  <si>
+    <t>userphonenumber</t>
+  </si>
+  <si>
+    <t>creditcardordebitcardnumber</t>
+  </si>
+  <si>
+    <t>expirationmonth</t>
+  </si>
+  <si>
+    <t>expirationyear</t>
+  </si>
+  <si>
+    <t>securiycode</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>Fifth</t>
+  </si>
+  <si>
+    <t>Sixth</t>
+  </si>
+  <si>
+    <t>Seventh</t>
+  </si>
+  <si>
+    <t>Eighth</t>
+  </si>
+  <si>
+    <t>Ninth</t>
+  </si>
+  <si>
+    <t>Tenth</t>
+  </si>
+  <si>
+    <t>Userone</t>
+  </si>
+  <si>
+    <t>Usertwo</t>
+  </si>
+  <si>
+    <t>Userthree</t>
+  </si>
+  <si>
+    <t>Userfour</t>
+  </si>
+  <si>
+    <t>Userfive</t>
+  </si>
+  <si>
+    <t>Usersix</t>
+  </si>
+  <si>
+    <t>Userseven</t>
+  </si>
+  <si>
+    <t>Usereight</t>
+  </si>
+  <si>
+    <t>Usernine</t>
+  </si>
+  <si>
+    <t>Userten</t>
+  </si>
+  <si>
+    <t>T Cedar Point Rd</t>
+  </si>
+  <si>
+    <t>Patuxent River</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>AB Goose Creek Resort</t>
+  </si>
+  <si>
+    <t>Newport</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>R Hensyn Vlg</t>
+  </si>
+  <si>
+    <t>Budd Lake</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>VC001 Woodfield Mall</t>
+  </si>
+  <si>
+    <t>Schaumburg</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>VC002 Woodfield Mall</t>
+  </si>
+  <si>
+    <t>user1@gmail.com</t>
+  </si>
+  <si>
+    <t>user2@gmail.com</t>
+  </si>
+  <si>
+    <t>user7@gmail.com</t>
+  </si>
+  <si>
+    <t>user3@gmail.com</t>
+  </si>
+  <si>
+    <t>user4@gmail.com</t>
+  </si>
+  <si>
+    <t>user5@gmail.com</t>
+  </si>
+  <si>
+    <t>user6@gmail.com</t>
+  </si>
+  <si>
+    <t>user8@gmailcom</t>
+  </si>
+  <si>
+    <t>user9@gmail.com</t>
+  </si>
+  <si>
+    <t>user10@gmail.com</t>
+  </si>
+  <si>
+    <t>980-563-1724</t>
+  </si>
+  <si>
+    <t>981-564-1725</t>
+  </si>
+  <si>
+    <t>981-564-1726</t>
+  </si>
+  <si>
+    <t>981-564-1727</t>
+  </si>
+  <si>
+    <t>981-564-1728</t>
+  </si>
+  <si>
+    <t>981-564-1730</t>
+  </si>
+  <si>
+    <t>981-564-1731</t>
+  </si>
+  <si>
+    <t>981-564-1732</t>
+  </si>
+  <si>
+    <t>981-564-1733</t>
+  </si>
+  <si>
+    <t>4263 9826 0269 5299</t>
+  </si>
+  <si>
+    <t>4264 9826 0269 5299</t>
+  </si>
+  <si>
+    <t>4265 9826 0269 5299</t>
+  </si>
+  <si>
+    <t>4266 9826 0269 5299</t>
+  </si>
+  <si>
+    <t>4267 9826 0269 5299</t>
+  </si>
+  <si>
+    <t>4268 9826 0269 5299</t>
+  </si>
+  <si>
+    <t>4270 9826 0269 5299</t>
+  </si>
+  <si>
+    <t>4271 9826 0269 5299</t>
+  </si>
+  <si>
+    <t>4272 9826 0269 5299</t>
+  </si>
+  <si>
+    <t>SearchBox</t>
+  </si>
+  <si>
+    <t>WD - My Passport Ultra for Mac 2TB External USB 3.0 Portable Hard Drive - Silver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +376,38 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFF9073B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF6A3E3E"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +438,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -202,10 +475,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -220,12 +494,59 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFE0000"/>
+      <color rgb="FFF9073B"/>
+      <color rgb="FFF20000"/>
+      <color rgb="FFFFC9C9"/>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -502,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M6" sqref="M4:M6"/>
     </sheetView>
   </sheetViews>
@@ -553,7 +874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -753,4 +1076,495 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="73.453125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.1796875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.90625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="21.08984375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="31.36328125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="18.6328125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.36328125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="14.36328125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="7">
+        <v>28570</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="7">
+        <v>2</v>
+      </c>
+      <c r="K2" s="7">
+        <v>2026</v>
+      </c>
+      <c r="L2" s="7">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="7">
+        <v>20670</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" s="7">
+        <v>4</v>
+      </c>
+      <c r="K3" s="7">
+        <v>2024</v>
+      </c>
+      <c r="L3" s="7">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="7">
+        <v>7828</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="7">
+        <v>6</v>
+      </c>
+      <c r="K4" s="7">
+        <v>2025</v>
+      </c>
+      <c r="L4" s="7">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="7">
+        <v>60173</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="7">
+        <v>8</v>
+      </c>
+      <c r="K5" s="7">
+        <v>2027</v>
+      </c>
+      <c r="L5" s="7">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="7">
+        <v>60173</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="7">
+        <v>10</v>
+      </c>
+      <c r="K6" s="7">
+        <v>2025</v>
+      </c>
+      <c r="L6" s="7">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="8">
+        <v>60173</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="8">
+        <v>3</v>
+      </c>
+      <c r="K7" s="8">
+        <v>2026</v>
+      </c>
+      <c r="L7" s="8">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="8">
+        <v>60174</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="8">
+        <v>5</v>
+      </c>
+      <c r="K8" s="8">
+        <v>2027</v>
+      </c>
+      <c r="L8" s="8">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="8">
+        <v>60175</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="8">
+        <v>2028</v>
+      </c>
+      <c r="L9" s="8">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="8">
+        <v>60176</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="8">
+        <v>8</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="8">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="8">
+        <v>60177</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="8">
+        <v>2</v>
+      </c>
+      <c r="K11" s="8">
+        <v>2026</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
+    <hyperlink ref="G11" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
This is seventh commit.
</commit_message>
<xml_diff>
--- a/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
+++ b/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,6 @@
     <sheet name="NavigateCheckoutAndDummyPayment" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1082,7 +1081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1110,7 +1109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
This is ninth commit.
</commit_message>
<xml_diff>
--- a/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
+++ b/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="SignUpTest" sheetId="2" r:id="rId2"/>
-    <sheet name="AddingItemToCart" sheetId="4" r:id="rId3"/>
-    <sheet name="NavigateCheckoutAndDummyPayment" sheetId="3" r:id="rId4"/>
+    <sheet name="ValidateTitleTest" sheetId="5" r:id="rId3"/>
+    <sheet name="AddingItemToCart" sheetId="4" r:id="rId4"/>
+    <sheet name="NavigateCheckoutAndDummyPayment" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1079,10 +1080,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="82.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1105,11 +1126,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
This is tenth commit.
</commit_message>
<xml_diff>
--- a/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
+++ b/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" tabRatio="828" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="SignUpTest" sheetId="2" r:id="rId2"/>
-    <sheet name="ValidateTitleTest" sheetId="5" r:id="rId3"/>
+    <sheet name="ValidateTitleTest" sheetId="7" r:id="rId2"/>
+    <sheet name="SignUpTest" sheetId="2" r:id="rId3"/>
     <sheet name="AddingItemToCart" sheetId="4" r:id="rId4"/>
     <sheet name="NavigateCheckoutAndDummyPayment" sheetId="3" r:id="rId5"/>
+    <sheet name="ValidateBottomLinks" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="186">
   <si>
     <t>Username</t>
   </si>
@@ -31,15 +32,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Prod</t>
-  </si>
-  <si>
     <t>Admin123</t>
   </si>
   <si>
@@ -121,9 +113,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">   </t>
-  </si>
-  <si>
     <t>firstName2</t>
   </si>
   <si>
@@ -347,13 +336,259 @@
   </si>
   <si>
     <t>WD - My Passport Ultra for Mac 2TB External USB 3.0 Portable Hard Drive - Silver</t>
+  </si>
+  <si>
+    <t>Gifts Cards and E-Gift Cards - Best Buy</t>
+  </si>
+  <si>
+    <t>Gift Ideas 2023: Best Gifts to Give This Year - Best Buy</t>
+  </si>
+  <si>
+    <t>Gift Ideas 2023: Best Gifts to Give This Year - Best Bui</t>
+  </si>
+  <si>
+    <t>emailaddress</t>
+  </si>
+  <si>
+    <t>stdentone@gmail.com</t>
+  </si>
+  <si>
+    <t>studenttwo@gmail.com</t>
+  </si>
+  <si>
+    <t>studentthree@gmail.com</t>
+  </si>
+  <si>
+    <t>studnetfour@gmail.com</t>
+  </si>
+  <si>
+    <t>studnetfive@gmail.com</t>
+  </si>
+  <si>
+    <t>studentsix@gmail.com</t>
+  </si>
+  <si>
+    <t>studentseven@gmail.com</t>
+  </si>
+  <si>
+    <t>studenteight@gmail.com</t>
+  </si>
+  <si>
+    <t>studentnine@gmail.com</t>
+  </si>
+  <si>
+    <t>studenten@gmail.com</t>
+  </si>
+  <si>
+    <t>Validate Bottom Links</t>
+  </si>
+  <si>
+    <t>Accessibility - Best Buy</t>
+  </si>
+  <si>
+    <t>BestBuy.com - Terms and Conditions</t>
+  </si>
+  <si>
+    <t>Privacy Policy Hub -  Best Buy</t>
+  </si>
+  <si>
+    <t>Interest-Based Ads - Best Buy</t>
+  </si>
+  <si>
+    <t>State Privacy Rights - Best Buy</t>
+  </si>
+  <si>
+    <t>Start Request - Best Buy</t>
+  </si>
+  <si>
+    <t>Best Buy</t>
+  </si>
+  <si>
+    <t>California Supply Chain Transperancy Act - Best Buy</t>
+  </si>
+  <si>
+    <t>Accessibility - Best Bui</t>
+  </si>
+  <si>
+    <t>BestBuy.com - Terms and Condition</t>
+  </si>
+  <si>
+    <t>Privacy Policy Hub -  Best Bui</t>
+  </si>
+  <si>
+    <t>Interest-Based Ads - Best Bui</t>
+  </si>
+  <si>
+    <t>State Privacy Rights - Best Bui</t>
+  </si>
+  <si>
+    <t>Start Request - Best Bui</t>
+  </si>
+  <si>
+    <t>Best Bui</t>
+  </si>
+  <si>
+    <t>California Supply Chain Transperancy Act - Best Bui</t>
+  </si>
+  <si>
+    <t>admin@login.com</t>
+  </si>
+  <si>
+    <t>invalidinput@.c</t>
+  </si>
+  <si>
+    <t>validinput@gmail.com</t>
+  </si>
+  <si>
+    <t>Title1</t>
+  </si>
+  <si>
+    <t>Title2</t>
+  </si>
+  <si>
+    <t>Title3</t>
+  </si>
+  <si>
+    <t>Title4</t>
+  </si>
+  <si>
+    <t>Sales and Promotions at Best Buy: On Sale Electronics, Coupons and Promo Codes</t>
+  </si>
+  <si>
+    <t>Sales and Promotions at Best Buy: On Sale Electronics, Coupons and Promo Code</t>
+  </si>
+  <si>
+    <t>Gifts Cards and E-Gift Cards - Best Bui</t>
+  </si>
+  <si>
+    <t>Title5</t>
+  </si>
+  <si>
+    <t>Title6</t>
+  </si>
+  <si>
+    <t>Top Deals and Featured Offers on Electronics - Best Buy</t>
+  </si>
+  <si>
+    <t>Title7</t>
+  </si>
+  <si>
+    <t>Title8</t>
+  </si>
+  <si>
+    <t>Top Deals and Featured Offers on Electronics - Best Bui</t>
+  </si>
+  <si>
+    <t>Deal of the Day: Electronics Deals - Best Buy</t>
+  </si>
+  <si>
+    <t>Title9</t>
+  </si>
+  <si>
+    <t>Title10</t>
+  </si>
+  <si>
+    <t>Title11</t>
+  </si>
+  <si>
+    <t>Title12</t>
+  </si>
+  <si>
+    <t>Title13</t>
+  </si>
+  <si>
+    <t>Title14</t>
+  </si>
+  <si>
+    <t>Title15</t>
+  </si>
+  <si>
+    <t>Title16</t>
+  </si>
+  <si>
+    <t>Title17</t>
+  </si>
+  <si>
+    <t>Title18</t>
+  </si>
+  <si>
+    <t>Title19</t>
+  </si>
+  <si>
+    <t>Title20</t>
+  </si>
+  <si>
+    <t>Title21</t>
+  </si>
+  <si>
+    <t>Title22</t>
+  </si>
+  <si>
+    <t>Yes, Best Buy Sells That – Best Buy</t>
+  </si>
+  <si>
+    <t>Yes, Best Buy Sells That – Best Bui</t>
+  </si>
+  <si>
+    <t>My Best Buy Memberships</t>
+  </si>
+  <si>
+    <t>My Best Buy Membership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Jude Childern's Research Hospital - Best Buy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Jude Childern's Research Hospital - Best Bui </t>
+  </si>
+  <si>
+    <t>Sign In to Best Buy</t>
+  </si>
+  <si>
+    <t>Sign In to Best Bui</t>
+  </si>
+  <si>
+    <t>Recently Viewed - Best Buy</t>
+  </si>
+  <si>
+    <t>Best Buy: Create an Account</t>
+  </si>
+  <si>
+    <t>Best Buy: Create a Account</t>
+  </si>
+  <si>
+    <t>Recently Viewed - Best Bui</t>
+  </si>
+  <si>
+    <t>Sign In for Order Status</t>
+  </si>
+  <si>
+    <t>Title23</t>
+  </si>
+  <si>
+    <t>Title24</t>
+  </si>
+  <si>
+    <t>Sign In for Order Statuses</t>
+  </si>
+  <si>
+    <t>Title25</t>
+  </si>
+  <si>
+    <t>Title26</t>
+  </si>
+  <si>
+    <t>Saved Items - Best Buy</t>
+  </si>
+  <si>
+    <t>Saved Items - Best Bui</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +637,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -479,7 +722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -530,6 +773,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -824,12 +1085,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M4:M6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
     <col min="2" max="2" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -842,234 +1103,234 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="63.36328125" customWidth="1"/>
+    <col min="2" max="2" width="63.1796875" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" customWidth="1"/>
+    <col min="5" max="5" width="42" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
+    <col min="7" max="7" width="43.36328125" customWidth="1"/>
+    <col min="8" max="8" width="43.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.1796875" customWidth="1"/>
+    <col min="10" max="10" width="34.36328125" customWidth="1"/>
+    <col min="11" max="11" width="26.81640625" customWidth="1"/>
+    <col min="12" max="12" width="27.453125" customWidth="1"/>
+    <col min="13" max="14" width="20.6328125" customWidth="1"/>
+    <col min="15" max="15" width="37.36328125" customWidth="1"/>
+    <col min="16" max="16" width="37.54296875" customWidth="1"/>
+    <col min="17" max="17" width="15.36328125" customWidth="1"/>
+    <col min="18" max="18" width="15.1796875" customWidth="1"/>
+    <col min="19" max="19" width="22.7265625" customWidth="1"/>
+    <col min="20" max="20" width="21.7265625" customWidth="1"/>
+    <col min="21" max="21" width="21.81640625" customWidth="1"/>
+    <col min="22" max="22" width="21.26953125" customWidth="1"/>
+    <col min="23" max="23" width="18.7265625" customWidth="1"/>
+    <col min="24" max="24" width="20.36328125" customWidth="1"/>
+    <col min="25" max="25" width="18.453125" customWidth="1"/>
+    <col min="26" max="26" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="4">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="4">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="4">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="4">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="5">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="5">
-        <v>9876</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="5">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="5">
-        <v>9876543211</v>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="V1" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="W1" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="X1" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y1" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z1" s="22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="R2" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="W2" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="X2" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y2" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1080,21 +1341,255 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="82.08984375" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="5">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5">
+        <v>9876</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="5">
+        <v>9876543211</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -1113,12 +1608,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1128,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1152,69 +1647,69 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F2" s="7">
         <v>28570</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J2" s="7">
         <v>2</v>
@@ -1228,31 +1723,31 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F3" s="7">
         <v>20670</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J3" s="7">
         <v>4</v>
@@ -1266,31 +1761,31 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F4" s="7">
         <v>7828</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J4" s="7">
         <v>6</v>
@@ -1304,31 +1799,31 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F5" s="7">
         <v>60173</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J5" s="7">
         <v>8</v>
@@ -1342,31 +1837,31 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F6" s="7">
         <v>60173</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J6" s="7">
         <v>10</v>
@@ -1380,31 +1875,31 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F7" s="8">
         <v>60173</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J7" s="8">
         <v>3</v>
@@ -1418,31 +1913,31 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F8" s="8">
         <v>60174</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J8" s="8">
         <v>5</v>
@@ -1456,34 +1951,34 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F9" s="8">
         <v>60175</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K9" s="8">
         <v>2028</v>
@@ -1494,37 +1989,37 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F10" s="8">
         <v>60176</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J10" s="8">
         <v>8</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L10" s="8">
         <v>884</v>
@@ -1532,31 +2027,31 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F11" s="8">
         <v>60177</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J11" s="8">
         <v>2</v>
@@ -1565,11 +2060,6 @@
         <v>2026</v>
       </c>
       <c r="L11" s="9"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F20" s="6" t="s">
-        <v>32</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1587,4 +2077,128 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="45.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
This is eleventh commit.
</commit_message>
<xml_diff>
--- a/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
+++ b/CapstoneOneBestBuyAutomation/data/CommonData.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="ValidateTitleTest" sheetId="7" r:id="rId2"/>
+    <sheet name="ValidateTitleTest1" sheetId="8" r:id="rId2"/>
     <sheet name="SignUpTest" sheetId="2" r:id="rId3"/>
     <sheet name="AddingItemToCart" sheetId="4" r:id="rId4"/>
     <sheet name="NavigateCheckoutAndDummyPayment" sheetId="3" r:id="rId5"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="189">
   <si>
     <t>Username</t>
   </si>
@@ -380,12 +380,6 @@
     <t>studenten@gmail.com</t>
   </si>
   <si>
-    <t>Validate Bottom Links</t>
-  </si>
-  <si>
-    <t>Accessibility - Best Buy</t>
-  </si>
-  <si>
     <t>BestBuy.com - Terms and Conditions</t>
   </si>
   <si>
@@ -407,9 +401,6 @@
     <t>California Supply Chain Transperancy Act - Best Buy</t>
   </si>
   <si>
-    <t>Accessibility - Best Bui</t>
-  </si>
-  <si>
     <t>BestBuy.com - Terms and Condition</t>
   </si>
   <si>
@@ -452,143 +443,161 @@
     <t>Title4</t>
   </si>
   <si>
+    <t>Sales and Promotions at Best Buy: On Sale Electronics, Coupons and Promo Code</t>
+  </si>
+  <si>
+    <t>Gifts Cards and E-Gift Cards - Best Bui</t>
+  </si>
+  <si>
+    <t>Title5</t>
+  </si>
+  <si>
+    <t>Title6</t>
+  </si>
+  <si>
+    <t>Top Deals and Featured Offers on Electronics - Best Buy</t>
+  </si>
+  <si>
+    <t>Title7</t>
+  </si>
+  <si>
+    <t>Title8</t>
+  </si>
+  <si>
+    <t>Top Deals and Featured Offers on Electronics - Best Bui</t>
+  </si>
+  <si>
+    <t>Deal of the Day: Electronics Deals - Best Buy</t>
+  </si>
+  <si>
+    <t>Title9</t>
+  </si>
+  <si>
+    <t>Title10</t>
+  </si>
+  <si>
+    <t>Title11</t>
+  </si>
+  <si>
+    <t>Title12</t>
+  </si>
+  <si>
+    <t>Title13</t>
+  </si>
+  <si>
+    <t>Title14</t>
+  </si>
+  <si>
+    <t>Title15</t>
+  </si>
+  <si>
+    <t>Title16</t>
+  </si>
+  <si>
+    <t>Title17</t>
+  </si>
+  <si>
+    <t>Title18</t>
+  </si>
+  <si>
+    <t>Title19</t>
+  </si>
+  <si>
+    <t>Title20</t>
+  </si>
+  <si>
+    <t>Title21</t>
+  </si>
+  <si>
+    <t>Title22</t>
+  </si>
+  <si>
+    <t>Yes, Best Buy Sells That – Best Buy</t>
+  </si>
+  <si>
+    <t>Yes, Best Buy Sells That – Best Bui</t>
+  </si>
+  <si>
+    <t>My Best Buy Memberships</t>
+  </si>
+  <si>
+    <t>My Best Buy Membership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Jude Childern's Research Hospital - Best Buy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">St. Jude Childern's Research Hospital - Best Bui </t>
+  </si>
+  <si>
+    <t>Sign In to Best Buy</t>
+  </si>
+  <si>
+    <t>Sign In to Best Bui</t>
+  </si>
+  <si>
+    <t>Recently Viewed - Best Buy</t>
+  </si>
+  <si>
+    <t>Best Buy: Create an Account</t>
+  </si>
+  <si>
+    <t>Best Buy: Create a Account</t>
+  </si>
+  <si>
+    <t>Recently Viewed - Best Bui</t>
+  </si>
+  <si>
+    <t>Sign In for Order Status</t>
+  </si>
+  <si>
+    <t>Title23</t>
+  </si>
+  <si>
+    <t>Title24</t>
+  </si>
+  <si>
+    <t>Sign In for Order Statuses</t>
+  </si>
+  <si>
+    <t>Title25</t>
+  </si>
+  <si>
+    <t>Title26</t>
+  </si>
+  <si>
+    <t>Saved Items - Best Buy</t>
+  </si>
+  <si>
+    <t>Saved Items - Best Bui</t>
+  </si>
+  <si>
     <t>Sales and Promotions at Best Buy: On Sale Electronics, Coupons and Promo Codes</t>
   </si>
   <si>
-    <t>Sales and Promotions at Best Buy: On Sale Electronics, Coupons and Promo Code</t>
-  </si>
-  <si>
-    <t>Gifts Cards and E-Gift Cards - Best Bui</t>
-  </si>
-  <si>
-    <t>Title5</t>
-  </si>
-  <si>
-    <t>Title6</t>
-  </si>
-  <si>
-    <t>Top Deals and Featured Offers on Electronics - Best Buy</t>
-  </si>
-  <si>
-    <t>Title7</t>
-  </si>
-  <si>
-    <t>Title8</t>
-  </si>
-  <si>
-    <t>Top Deals and Featured Offers on Electronics - Best Bui</t>
-  </si>
-  <si>
-    <t>Deal of the Day: Electronics Deals - Best Buy</t>
-  </si>
-  <si>
-    <t>Title9</t>
-  </si>
-  <si>
-    <t>Title10</t>
-  </si>
-  <si>
-    <t>Title11</t>
-  </si>
-  <si>
-    <t>Title12</t>
-  </si>
-  <si>
-    <t>Title13</t>
-  </si>
-  <si>
-    <t>Title14</t>
-  </si>
-  <si>
-    <t>Title15</t>
-  </si>
-  <si>
-    <t>Title16</t>
-  </si>
-  <si>
-    <t>Title17</t>
-  </si>
-  <si>
-    <t>Title18</t>
-  </si>
-  <si>
-    <t>Title19</t>
-  </si>
-  <si>
-    <t>Title20</t>
-  </si>
-  <si>
-    <t>Title21</t>
-  </si>
-  <si>
-    <t>Title22</t>
-  </si>
-  <si>
-    <t>Yes, Best Buy Sells That – Best Buy</t>
-  </si>
-  <si>
-    <t>Yes, Best Buy Sells That – Best Bui</t>
-  </si>
-  <si>
-    <t>My Best Buy Memberships</t>
-  </si>
-  <si>
-    <t>My Best Buy Membership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Jude Childern's Research Hospital - Best Buy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Jude Childern's Research Hospital - Best Bui </t>
-  </si>
-  <si>
-    <t>Sign In to Best Buy</t>
-  </si>
-  <si>
-    <t>Sign In to Best Bui</t>
-  </si>
-  <si>
-    <t>Recently Viewed - Best Buy</t>
-  </si>
-  <si>
-    <t>Best Buy: Create an Account</t>
-  </si>
-  <si>
-    <t>Best Buy: Create a Account</t>
-  </si>
-  <si>
-    <t>Recently Viewed - Best Bui</t>
-  </si>
-  <si>
-    <t>Sign In for Order Status</t>
-  </si>
-  <si>
-    <t>Title23</t>
-  </si>
-  <si>
-    <t>Title24</t>
-  </si>
-  <si>
-    <t>Sign In for Order Statuses</t>
-  </si>
-  <si>
-    <t>Title25</t>
-  </si>
-  <si>
-    <t>Title26</t>
-  </si>
-  <si>
-    <t>Saved Items - Best Buy</t>
-  </si>
-  <si>
-    <t>Saved Items - Best Bui</t>
+    <t>Deal of the Day: Electronics Deals - Best Bui</t>
+  </si>
+  <si>
+    <t>St. Jude Children&amp;#x27;s Research Hospital - Best Buy</t>
+  </si>
+  <si>
+    <t>Best Buy: Create an Accounts</t>
+  </si>
+  <si>
+    <t>Sign In for Order Statu</t>
+  </si>
+  <si>
+    <t>Accessibility Best Buy</t>
+  </si>
+  <si>
+    <t>Accessibility Best Bui</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -642,12 +651,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color theme="4" tint="-0.499984740745262"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -694,7 +708,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -717,12 +731,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -773,9 +800,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -783,14 +807,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1085,7 +1115,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1103,24 +1133,24 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>135</v>
+      <c r="A2" s="20" t="s">
+        <v>132</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
-        <v>136</v>
+      <c r="A3" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
-        <v>137</v>
+      <c r="A4" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1141,196 +1171,196 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+      <selection sqref="A1:Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.36328125" customWidth="1"/>
-    <col min="2" max="2" width="63.1796875" customWidth="1"/>
-    <col min="3" max="3" width="30.26953125" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" customWidth="1"/>
-    <col min="5" max="5" width="42" customWidth="1"/>
-    <col min="6" max="6" width="48" customWidth="1"/>
-    <col min="7" max="7" width="43.36328125" customWidth="1"/>
-    <col min="8" max="8" width="43.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.1796875" customWidth="1"/>
-    <col min="10" max="10" width="34.36328125" customWidth="1"/>
-    <col min="11" max="11" width="26.81640625" customWidth="1"/>
-    <col min="12" max="12" width="27.453125" customWidth="1"/>
-    <col min="13" max="14" width="20.6328125" customWidth="1"/>
-    <col min="15" max="15" width="37.36328125" customWidth="1"/>
-    <col min="16" max="16" width="37.54296875" customWidth="1"/>
-    <col min="17" max="17" width="15.36328125" customWidth="1"/>
-    <col min="18" max="18" width="15.1796875" customWidth="1"/>
-    <col min="19" max="19" width="22.7265625" customWidth="1"/>
-    <col min="20" max="20" width="21.7265625" customWidth="1"/>
-    <col min="21" max="21" width="21.81640625" customWidth="1"/>
-    <col min="22" max="22" width="21.26953125" customWidth="1"/>
-    <col min="23" max="23" width="18.7265625" customWidth="1"/>
-    <col min="24" max="24" width="20.36328125" customWidth="1"/>
-    <col min="25" max="25" width="18.453125" customWidth="1"/>
-    <col min="26" max="26" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="122.1796875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="121.90625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="61.1796875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="61.90625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="87.36328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="87.6328125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="85.81640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="86.81640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="70.81640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="71.26953125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="54.81640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="55.08984375" style="6" customWidth="1"/>
+    <col min="13" max="14" width="36.26953125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="83.08984375" style="6" customWidth="1"/>
+    <col min="16" max="16" width="83.36328125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="30.453125" style="6" customWidth="1"/>
+    <col min="18" max="18" width="30.6328125" style="6" customWidth="1"/>
+    <col min="19" max="19" width="43.36328125" style="6" customWidth="1"/>
+    <col min="20" max="20" width="44.453125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="41.90625" style="6" customWidth="1"/>
+    <col min="22" max="22" width="43.26953125" style="6" customWidth="1"/>
+    <col min="23" max="23" width="37.90625" style="6" customWidth="1"/>
+    <col min="24" max="24" width="38" style="6" customWidth="1"/>
+    <col min="25" max="25" width="35.1796875" customWidth="1"/>
+    <col min="26" max="26" width="34.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="E1" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="X1" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C2" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="22" t="s">
+      <c r="E2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="G1" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="R1" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="S1" s="22" t="s">
+      <c r="I2" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="K2" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="L2" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="M2" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="V1" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="W1" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="X1" s="22" t="s">
+      <c r="N2" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="S2" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="T2" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="U2" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="W2" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="X2" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y2" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="Y1" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z1" s="22" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="P2" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q2" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="R2" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="T2" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="U2" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="V2" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="W2" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="X2" s="23" t="s">
+      <c r="Z2" s="27" t="s">
         <v>181</v>
-      </c>
-      <c r="Y2" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z2" s="23" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1414,7 @@
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>108</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1404,7 +1434,7 @@
       <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>109</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1424,7 +1454,7 @@
       <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>110</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1444,7 +1474,7 @@
       <c r="B5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>111</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1464,7 +1494,7 @@
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>112</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1484,7 +1514,7 @@
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>113</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1502,7 +1532,7 @@
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -1522,7 +1552,7 @@
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>115</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1542,7 +1572,7 @@
       <c r="B10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>116</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1562,7 +1592,7 @@
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>117</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1626,7 +1656,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:L11"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2081,120 +2111,318 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A21"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection sqref="A1:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.453125" customWidth="1"/>
+    <col min="1" max="1" width="35.08984375" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" customWidth="1"/>
+    <col min="3" max="3" width="53.54296875" customWidth="1"/>
+    <col min="4" max="4" width="51.81640625" customWidth="1"/>
+    <col min="5" max="5" width="47.1796875" customWidth="1"/>
+    <col min="6" max="6" width="46.90625" customWidth="1"/>
+    <col min="7" max="7" width="46.81640625" customWidth="1"/>
+    <col min="8" max="8" width="45.1796875" customWidth="1"/>
+    <col min="9" max="9" width="49.7265625" customWidth="1"/>
+    <col min="10" max="10" width="48.7265625" customWidth="1"/>
+    <col min="11" max="11" width="47.81640625" customWidth="1"/>
+    <col min="12" max="12" width="47.08984375" customWidth="1"/>
+    <col min="13" max="13" width="38.08984375" customWidth="1"/>
+    <col min="14" max="14" width="37.90625" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" customWidth="1"/>
+    <col min="16" max="16" width="14.26953125" customWidth="1"/>
+    <col min="17" max="17" width="38.36328125" customWidth="1"/>
+    <col min="18" max="18" width="38.6328125" customWidth="1"/>
+    <col min="19" max="19" width="80" customWidth="1"/>
+    <col min="20" max="20" width="80.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="D2" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="F2" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="28" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="I2" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="K2" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" s="28" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="O2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q2" s="28" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="R2" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="T2" s="28" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>134</v>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A31" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="I31" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="K31" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="L31" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="N31" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O31" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="P31" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q31" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="R31" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="S31" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="T31" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="U31" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="V31" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="W31" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="X31" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y31" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z31" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A32" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="H32" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="I32" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="J32" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="K32" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="L32" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="M32" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="N32" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="O32" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="P32" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q32" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="R32" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="S32" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="T32" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="U32" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="V32" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="W32" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="X32" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y32" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z32" s="24" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>